<commit_message>
Doc(jdt) jdt du 07.11.2025
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cours\P_bulle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3FE41D-C57A-4154-8103-6C6C8BC88517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A661B9D7-AEE7-4E19-B4E9-26AB59B9B919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>Auteur:</t>
   </si>
@@ -139,7 +139,25 @@
     <t>hello-world</t>
   </si>
   <si>
-    <t>13h24</t>
+    <t>13h24-13h32</t>
+  </si>
+  <si>
+    <t>annalyns-infiltration</t>
+  </si>
+  <si>
+    <t>13h39-15h11  (-15min de pause)</t>
+  </si>
+  <si>
+    <t>Lasagna</t>
+  </si>
+  <si>
+    <t>15h15-16h03</t>
+  </si>
+  <si>
+    <t>freelancer-rates</t>
+  </si>
+  <si>
+    <t>16h07-16h30</t>
   </si>
 </sst>
 </file>
@@ -1082,7 +1100,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>175</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1934,7 +1952,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4126,7 +4144,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4181,7 +4199,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>0 heures 0 minutes</v>
+        <v>2 heures 55 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4196,15 +4214,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4247,7 +4265,9 @@
         <v>45968</v>
       </c>
       <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
+      <c r="D7" s="34">
+        <v>10</v>
+      </c>
       <c r="E7" s="35" t="s">
         <v>19</v>
       </c>
@@ -4259,16 +4279,28 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="73" t="str">
+      <c r="A8" s="73">
         <f>IF(ISBLANK(B8),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B8))</f>
-        <v/>
-      </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="45"/>
+        <v>45</v>
+      </c>
+      <c r="B8" s="36">
+        <v>45968</v>
+      </c>
+      <c r="C8" s="37">
+        <v>1</v>
+      </c>
+      <c r="D8" s="38">
+        <v>30</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="45" t="s">
+        <v>34</v>
+      </c>
       <c r="M8" t="s">
         <v>2</v>
       </c>
@@ -4280,16 +4312,26 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="74" t="str">
+      <c r="A9" s="74">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v/>
-      </c>
-      <c r="B9" s="40"/>
+        <v>45</v>
+      </c>
+      <c r="B9" s="40">
+        <v>45968</v>
+      </c>
       <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="46"/>
+      <c r="D9" s="42">
+        <v>50</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>36</v>
+      </c>
       <c r="M9" t="s">
         <v>19</v>
       </c>
@@ -4301,16 +4343,26 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="73" t="str">
+      <c r="A10" s="73">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="36"/>
+        <v>45</v>
+      </c>
+      <c r="B10" s="36">
+        <v>45968</v>
+      </c>
       <c r="C10" s="37"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="45"/>
+      <c r="D10" s="38">
+        <v>25</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="45" t="s">
+        <v>38</v>
+      </c>
       <c r="M10" t="s">
         <v>3</v>
       </c>
@@ -10784,9 +10836,9 @@
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
         <v>0 h 00 min</v>
       </c>
-      <c r="G6" s="47" t="e">
+      <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10803,15 +10855,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10819,11 +10871,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>0 h 00 min</v>
-      </c>
-      <c r="G7" s="56" t="e">
+        <v>2 h 55 min</v>
+      </c>
+      <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10858,9 +10910,9 @@
         <f t="shared" si="1"/>
         <v>0 h 00 min</v>
       </c>
-      <c r="G8" s="47" t="e">
+      <c r="G8" s="47">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L8" s="65" t="str">
         <f>'Journal de travail'!M10</f>
@@ -10895,9 +10947,9 @@
         <f t="shared" si="1"/>
         <v>0 h 00 min</v>
       </c>
-      <c r="G9" s="56" t="e">
+      <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -10914,26 +10966,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>0 h 00 min</v>
+        <v>2 h 55 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0</v>
+        <v>3.3143939393939392E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Doc(jdt) jdt du 14.11.2025
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cours\P_bulle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\py13koy\Documents\github\p-bulle-exercices-js-start\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A661B9D7-AEE7-4E19-B4E9-26AB59B9B919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5721A1-8397-4705-9C6E-A64860A725C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>Auteur:</t>
   </si>
@@ -157,7 +157,40 @@
     <t>freelancer-rates</t>
   </si>
   <si>
-    <t>16h07-16h30</t>
+    <t>16h07-16h30 WIP</t>
+  </si>
+  <si>
+    <t>12h36-13h25</t>
+  </si>
+  <si>
+    <t>poetry-club-door-policy</t>
+  </si>
+  <si>
+    <t>13h26-14h45</t>
+  </si>
+  <si>
+    <t>freelancer-rates améloration</t>
+  </si>
+  <si>
+    <t>15h08-15h15</t>
+  </si>
+  <si>
+    <t>elyses-enchantments</t>
+  </si>
+  <si>
+    <t>15h21-15h55</t>
+  </si>
+  <si>
+    <t>freelancer-rates/poetry-club-door-policy/elyses-enchantments amélioration</t>
+  </si>
+  <si>
+    <t>16h12-16h19</t>
+  </si>
+  <si>
+    <t>16h22-16h30</t>
+  </si>
+  <si>
+    <t>lecture de vehicle-purchase</t>
   </si>
 </sst>
 </file>
@@ -1097,10 +1130,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>175</c:v>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1949,10 +1982,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2.7777777777777776E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.97222222222222221</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4144,7 +4177,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4199,7 +4232,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>2 heures 55 minutes</v>
+        <v>6 heures 0 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4214,15 +4247,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>115</v>
+        <v>240</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>175</v>
+        <v>360</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4374,16 +4407,26 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="str">
+      <c r="A11" s="74">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="40"/>
+        <v>46</v>
+      </c>
+      <c r="B11" s="40">
+        <v>45975</v>
+      </c>
       <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="46"/>
+      <c r="D11" s="42">
+        <v>50</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="46" t="s">
+        <v>39</v>
+      </c>
       <c r="M11" t="s">
         <v>4</v>
       </c>
@@ -4395,16 +4438,28 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="73" t="str">
+      <c r="A12" s="73">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="45"/>
+        <v>46</v>
+      </c>
+      <c r="B12" s="36">
+        <v>45975</v>
+      </c>
+      <c r="C12" s="37">
+        <v>1</v>
+      </c>
+      <c r="D12" s="38">
+        <v>20</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="45" t="s">
+        <v>41</v>
+      </c>
       <c r="N12">
         <v>5</v>
       </c>
@@ -4413,16 +4468,26 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="74" t="str">
+      <c r="A13" s="74">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="40"/>
+        <v>46</v>
+      </c>
+      <c r="B13" s="40">
+        <v>45975</v>
+      </c>
       <c r="C13" s="41"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="46"/>
+      <c r="D13" s="42">
+        <v>5</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="46" t="s">
+        <v>43</v>
+      </c>
       <c r="N13">
         <v>6</v>
       </c>
@@ -4431,16 +4496,26 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="73" t="str">
+      <c r="A14" s="73">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="36"/>
+        <v>46</v>
+      </c>
+      <c r="B14" s="36">
+        <v>45975</v>
+      </c>
       <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="45"/>
+      <c r="D14" s="38">
+        <v>35</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="45" t="s">
+        <v>45</v>
+      </c>
       <c r="N14">
         <v>7</v>
       </c>
@@ -4449,16 +4524,26 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="74" t="str">
+      <c r="A15" s="74">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="40"/>
+        <v>46</v>
+      </c>
+      <c r="B15" s="40">
+        <v>45975</v>
+      </c>
       <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="46"/>
+      <c r="D15" s="42">
+        <v>5</v>
+      </c>
+      <c r="E15" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="46" t="s">
+        <v>47</v>
+      </c>
       <c r="N15">
         <v>8</v>
       </c>
@@ -4467,16 +4552,26 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="73" t="str">
+      <c r="A16" s="73">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="36"/>
+        <v>46</v>
+      </c>
+      <c r="B16" s="36">
+        <v>45975</v>
+      </c>
       <c r="C16" s="37"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="45"/>
+      <c r="D16" s="38">
+        <v>10</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="45" t="s">
+        <v>48</v>
+      </c>
       <c r="O16">
         <v>40</v>
       </c>
@@ -10822,11 +10917,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C9" si="0">SUM(A6:B6)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10834,11 +10929,11 @@
       </c>
       <c r="F6" s="50" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>0 h 00 min</v>
+        <v>0 h 10 min</v>
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0</v>
+        <v>2.7777777777777776E-2</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10855,15 +10950,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>115</v>
+        <v>230</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>175</v>
+        <v>350</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10871,11 +10966,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>2 h 55 min</v>
+        <v>5 h 50 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>1</v>
+        <v>0.97222222222222221</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10966,26 +11061,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>115</v>
+        <v>240</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>175</v>
+        <v>360</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>2 h 55 min</v>
+        <v>6 h 00 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>3.3143939393939392E-2</v>
+        <v>6.8181818181818177E-2</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11029,27 +11124,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="020ab319e6f8d23aec07c29d6516d4ba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e15d3f914bf2a775f9387e5284d9197" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11262,10 +11336,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6394C10-4386-493D-A99B-15992834CB10}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11284,20 +11390,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6394C10-4386-493D-A99B-15992834CB10}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DOC(jdt) jdt du 21.11.2025
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\py13koy\Documents\github\p-bulle-exercices-js-start\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5721A1-8397-4705-9C6E-A64860A725C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FB0024-6634-47D0-8892-AC686A156001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
   <si>
     <t>Auteur:</t>
   </si>
@@ -191,6 +191,36 @@
   </si>
   <si>
     <t>lecture de vehicle-purchase</t>
+  </si>
+  <si>
+    <t>vehicle-purchase</t>
+  </si>
+  <si>
+    <t>12h30-12h53</t>
+  </si>
+  <si>
+    <t>amusement-park</t>
+  </si>
+  <si>
+    <t>elyses-looping-enchantments</t>
+  </si>
+  <si>
+    <t>13h04-13h21 WIP</t>
+  </si>
+  <si>
+    <t>13h35-14h17</t>
+  </si>
+  <si>
+    <t>space-age</t>
+  </si>
+  <si>
+    <t>14h22-16h   (-15min de pause)</t>
+  </si>
+  <si>
+    <t>fruit-picker</t>
+  </si>
+  <si>
+    <t>16h11-16h35 WIP</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1163,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>350</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1982,10 +2012,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.7777777777777776E-2</c:v>
+                  <c:v>1.7857142857142856E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.97222222222222221</c:v>
+                  <c:v>0.9821428571428571</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4175,9 +4205,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4232,7 +4262,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>6 heures 0 minutes</v>
+        <v>9 heures 20 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4247,15 +4277,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>240</v>
+        <v>380</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>360</v>
+        <v>560</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4577,73 +4607,125 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="74" t="str">
+      <c r="A17" s="74">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="40"/>
+        <v>47</v>
+      </c>
+      <c r="B17" s="40">
+        <v>45982</v>
+      </c>
       <c r="C17" s="41"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="46"/>
+      <c r="D17" s="42">
+        <v>25</v>
+      </c>
+      <c r="E17" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="46" t="s">
+        <v>51</v>
+      </c>
       <c r="O17">
         <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="73" t="str">
+      <c r="A18" s="73">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="36"/>
+        <v>47</v>
+      </c>
+      <c r="B18" s="36">
+        <v>45982</v>
+      </c>
       <c r="C18" s="37"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="45"/>
+      <c r="D18" s="38">
+        <v>15</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="45" t="s">
+        <v>54</v>
+      </c>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="74" t="str">
+      <c r="A19" s="74">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="40"/>
+        <v>47</v>
+      </c>
+      <c r="B19" s="40">
+        <v>45982</v>
+      </c>
       <c r="C19" s="41"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="46"/>
+      <c r="D19" s="42">
+        <v>40</v>
+      </c>
+      <c r="E19" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="46" t="s">
+        <v>55</v>
+      </c>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="73" t="str">
+      <c r="A20" s="73">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="45"/>
+        <v>47</v>
+      </c>
+      <c r="B20" s="36">
+        <v>45982</v>
+      </c>
+      <c r="C20" s="37">
+        <v>1</v>
+      </c>
+      <c r="D20" s="38">
+        <v>40</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="45" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="74" t="str">
+      <c r="A21" s="74">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="40"/>
+        <v>47</v>
+      </c>
+      <c r="B21" s="40">
+        <v>45982</v>
+      </c>
       <c r="C21" s="41"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="46"/>
+      <c r="D21" s="42">
+        <v>20</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="46" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="73" t="str">
@@ -10933,7 +11015,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>2.7777777777777776E-2</v>
+        <v>1.7857142857142856E-2</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10950,15 +11032,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>230</v>
+        <v>370</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>350</v>
+        <v>550</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -10966,11 +11048,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>5 h 50 min</v>
+        <v>9 h 10 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.97222222222222221</v>
+        <v>0.9821428571428571</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11061,26 +11143,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>240</v>
+        <v>380</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>360</v>
+        <v>560</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>6 h 00 min</v>
+        <v>9 h 20 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>6.8181818181818177E-2</v>
+        <v>0.10606060606060606</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11124,6 +11206,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="020ab319e6f8d23aec07c29d6516d4ba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e15d3f914bf2a775f9387e5284d9197" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11336,42 +11439,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6394C10-4386-493D-A99B-15992834CB10}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11390,9 +11461,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6394C10-4386-493D-A99B-15992834CB10}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DOC(jdt) jdt du 28.11.2025
[DONE]
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\py13koy\Documents\github\p-bulle-exercices-js-start\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FB0024-6634-47D0-8892-AC686A156001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C676EC-5EC5-4657-80E8-BEBEFCACB2F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="65">
   <si>
     <t>Auteur:</t>
   </si>
@@ -221,6 +221,21 @@
   </si>
   <si>
     <t>16h11-16h35 WIP</t>
+  </si>
+  <si>
+    <t>space-age amélioration</t>
+  </si>
+  <si>
+    <t>12h26-12h37</t>
+  </si>
+  <si>
+    <t>12h39-13h01</t>
+  </si>
+  <si>
+    <t>13h04-14h13</t>
+  </si>
+  <si>
+    <t>14h17-16h22 (-20min de pause)</t>
   </si>
 </sst>
 </file>
@@ -455,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -650,6 +665,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1163,7 +1182,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>550</c:v>
+                  <c:v>775</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2012,10 +2031,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.7857142857142856E-2</c:v>
+                  <c:v>1.2738853503184714E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9821428571428571</c:v>
+                  <c:v>0.98726114649681529</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4205,9 +4224,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4262,7 +4281,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>9 heures 20 minutes</v>
+        <v>13 heures 5 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4277,15 +4296,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>380</v>
+        <v>425</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>560</v>
+        <v>785</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4728,52 +4747,96 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="73" t="str">
+      <c r="A22" s="73">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="36"/>
+        <v>48</v>
+      </c>
+      <c r="B22" s="36">
+        <v>45989</v>
+      </c>
       <c r="C22" s="37"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="45"/>
+      <c r="D22" s="38">
+        <v>10</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" s="83" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="74" t="str">
+      <c r="A23" s="74">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="40"/>
+        <v>48</v>
+      </c>
+      <c r="B23" s="40">
+        <v>45989</v>
+      </c>
       <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="46"/>
+      <c r="D23" s="42">
+        <v>20</v>
+      </c>
+      <c r="E23" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" s="46" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="73" t="str">
+      <c r="A24" s="73">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="45"/>
+        <v>48</v>
+      </c>
+      <c r="B24" s="36">
+        <v>45989</v>
+      </c>
+      <c r="C24" s="37">
+        <v>1</v>
+      </c>
+      <c r="D24" s="38">
+        <v>10</v>
+      </c>
+      <c r="E24" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="45" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="74" t="str">
+      <c r="A25" s="74">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="46"/>
+        <v>48</v>
+      </c>
+      <c r="B25" s="40">
+        <v>45989</v>
+      </c>
+      <c r="C25" s="41">
+        <v>2</v>
+      </c>
+      <c r="D25" s="42">
+        <v>5</v>
+      </c>
+      <c r="E25" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="46" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="73" t="str">
@@ -11015,7 +11078,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>1.7857142857142856E-2</v>
+        <v>1.2738853503184714E-2</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11032,15 +11095,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>370</v>
+        <v>415</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>550</v>
+        <v>775</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11048,11 +11111,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>9 h 10 min</v>
+        <v>12 h 55 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.9821428571428571</v>
+        <v>0.98726114649681529</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11143,26 +11206,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>180</v>
+        <v>360</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>380</v>
+        <v>425</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>560</v>
+        <v>785</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>9 h 20 min</v>
+        <v>13 h 05 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.10606060606060606</v>
+        <v>0.14867424242424243</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11206,27 +11269,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="020ab319e6f8d23aec07c29d6516d4ba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e15d3f914bf2a775f9387e5284d9197" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11439,10 +11481,42 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6394C10-4386-493D-A99B-15992834CB10}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11461,20 +11535,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6394C10-4386-493D-A99B-15992834CB10}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DOC(jdt) jdt du 05.12.2025
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\py13koy\Documents\github\p-bulle-exercices-js-start\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C676EC-5EC5-4657-80E8-BEBEFCACB2F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDE98C3-D30C-4455-A1F2-0BC6D3737AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="76">
   <si>
     <t>Auteur:</t>
   </si>
@@ -236,6 +236,39 @@
   </si>
   <si>
     <t>14h17-16h22 (-20min de pause)</t>
+  </si>
+  <si>
+    <t>13h03-13h31</t>
+  </si>
+  <si>
+    <t>bank-account</t>
+  </si>
+  <si>
+    <t>13h37-14h21</t>
+  </si>
+  <si>
+    <t>amusement-park amélioration</t>
+  </si>
+  <si>
+    <t>14h24-14h29</t>
+  </si>
+  <si>
+    <t>captains-log</t>
+  </si>
+  <si>
+    <t>14h34-15h28 (-20min de pause)</t>
+  </si>
+  <si>
+    <t>gigasecond</t>
+  </si>
+  <si>
+    <t>15h33-16h01</t>
+  </si>
+  <si>
+    <t>compréhension lucky-number intro</t>
+  </si>
+  <si>
+    <t>16h05-16h15 WIP</t>
   </si>
 </sst>
 </file>
@@ -656,6 +689,10 @@
       <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="16" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -665,10 +702,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1179,10 +1212,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>775</c:v>
+                  <c:v>920</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2031,10 +2064,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.2738853503184714E-2</c:v>
+                  <c:v>2.1276595744680851E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98726114649681529</c:v>
+                  <c:v>0.97872340425531912</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -4224,9 +4257,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4258,15 +4291,15 @@
       <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="80" t="s">
+      <c r="B2" s="83"/>
+      <c r="C2" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
       <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
@@ -4275,13 +4308,13 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="82"/>
+      <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>13 heures 5 minutes</v>
+        <v>15 heures 40 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4300,20 +4333,20 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>425</v>
+        <v>580</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>785</v>
+        <v>940</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="81" t="s">
+      <c r="C5" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="81"/>
+      <c r="D5" s="82"/>
     </row>
     <row r="6" spans="1:15" s="17" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
@@ -4764,7 +4797,7 @@
       <c r="F22" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="G22" s="83" t="s">
+      <c r="G22" s="80" t="s">
         <v>61</v>
       </c>
     </row>
@@ -4839,76 +4872,136 @@
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="73" t="str">
+      <c r="A26" s="73">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v/>
-      </c>
-      <c r="B26" s="36"/>
+        <v>49</v>
+      </c>
+      <c r="B26" s="36">
+        <v>45996</v>
+      </c>
       <c r="C26" s="37"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="45"/>
+      <c r="D26" s="38">
+        <v>30</v>
+      </c>
+      <c r="E26" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="G26" s="45" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="74" t="str">
+      <c r="A27" s="74">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="40"/>
+        <v>49</v>
+      </c>
+      <c r="B27" s="40">
+        <v>45996</v>
+      </c>
       <c r="C27" s="41"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="46"/>
+      <c r="D27" s="42">
+        <v>45</v>
+      </c>
+      <c r="E27" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" s="46" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="73" t="str">
+      <c r="A28" s="73">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="36"/>
+        <v>49</v>
+      </c>
+      <c r="B28" s="36">
+        <v>45996</v>
+      </c>
       <c r="C28" s="37"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="45"/>
+      <c r="D28" s="38">
+        <v>5</v>
+      </c>
+      <c r="E28" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" s="45" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="74" t="str">
+      <c r="A29" s="74">
         <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B29))</f>
-        <v/>
-      </c>
-      <c r="B29" s="40"/>
+        <v>49</v>
+      </c>
+      <c r="B29" s="40">
+        <v>45996</v>
+      </c>
       <c r="C29" s="41"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="46"/>
+      <c r="D29" s="42">
+        <v>35</v>
+      </c>
+      <c r="E29" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" s="46" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="73" t="str">
+      <c r="A30" s="73">
         <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B30))</f>
-        <v/>
-      </c>
-      <c r="B30" s="36"/>
+        <v>49</v>
+      </c>
+      <c r="B30" s="36">
+        <v>45996</v>
+      </c>
       <c r="C30" s="37"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="45"/>
+      <c r="D30" s="38">
+        <v>30</v>
+      </c>
+      <c r="E30" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G30" s="45" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="74" t="str">
+      <c r="A31" s="74">
         <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B31))</f>
-        <v/>
-      </c>
-      <c r="B31" s="40"/>
+        <v>49</v>
+      </c>
+      <c r="B31" s="40">
+        <v>45996</v>
+      </c>
       <c r="C31" s="41"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="46"/>
+      <c r="D31" s="42">
+        <v>10</v>
+      </c>
+      <c r="E31" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="G31" s="46" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="73" t="str">
@@ -11062,11 +11155,11 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <f t="shared" ref="C6:C9" si="0">SUM(A6:B6)</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E6" s="21" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11074,11 +11167,11 @@
       </c>
       <c r="F6" s="50" t="str">
         <f>QUOTIENT(SUM(A6:B6),60)&amp;" h "&amp;TEXT(MOD(SUM(A6:B6),60), "00")&amp;" min"</f>
-        <v>0 h 10 min</v>
+        <v>0 h 20 min</v>
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>1.2738853503184714E-2</v>
+        <v>2.1276595744680851E-2</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11099,11 +11192,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>415</v>
+        <v>560</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>775</v>
+        <v>920</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11111,11 +11204,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>12 h 55 min</v>
+        <v>15 h 20 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.98726114649681529</v>
+        <v>0.97872340425531912</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11210,22 +11303,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>425</v>
+        <v>580</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>785</v>
+        <v>940</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>13 h 05 min</v>
+        <v>15 h 40 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.14867424242424243</v>
+        <v>0.17803030303030304</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11269,6 +11362,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="020ab319e6f8d23aec07c29d6516d4ba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e15d3f914bf2a775f9387e5284d9197" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11481,42 +11595,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6394C10-4386-493D-A99B-15992834CB10}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11535,9 +11617,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6394C10-4386-493D-A99B-15992834CB10}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DOC(jdt) jdt du 19.12.2025
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\py13koy\Documents\github\p-bulle-exercices-js-start\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA2CD5E-79E4-4707-8811-7560D52BEECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7654E6-27C7-4B8F-8CFD-770214983F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="106">
   <si>
     <t>Auteur:</t>
   </si>
@@ -311,6 +311,54 @@
   </si>
   <si>
     <t>16h24-16h27</t>
+  </si>
+  <si>
+    <t>10h54-11h02</t>
+  </si>
+  <si>
+    <t>Réinstalation du tool-set</t>
+  </si>
+  <si>
+    <t>bank-account et lucky-numbers amélioration</t>
+  </si>
+  <si>
+    <t>12h28-12h42</t>
+  </si>
+  <si>
+    <t>elyses-destructured-enchantment</t>
+  </si>
+  <si>
+    <t>12h46-13h39</t>
+  </si>
+  <si>
+    <t>bob</t>
+  </si>
+  <si>
+    <t>13h43-14h04</t>
+  </si>
+  <si>
+    <t>mixed-juces</t>
+  </si>
+  <si>
+    <t>14h09-14h44</t>
+  </si>
+  <si>
+    <t>15h04-15h05</t>
+  </si>
+  <si>
+    <t>vehicle-purchase amélioration</t>
+  </si>
+  <si>
+    <t>bird-watcher</t>
+  </si>
+  <si>
+    <t>15h08-15h30</t>
+  </si>
+  <si>
+    <t>elyses-analytic-enchantment</t>
+  </si>
+  <si>
+    <t>15h37-15h59</t>
   </si>
 </sst>
 </file>
@@ -1257,7 +1305,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1085</c:v>
+                  <c:v>1240</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>40</c:v>
@@ -2106,13 +2154,13 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.7467248908296942E-2</c:v>
+                  <c:v>1.5384615384615385E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.94759825327510916</c:v>
+                  <c:v>0.9538461538461539</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.4934497816593885E-2</c:v>
+                  <c:v>3.0769230769230771E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -4300,8 +4348,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B41" sqref="B41"/>
+      <pane ySplit="6" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4356,7 +4404,7 @@
       <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>19 heures 5 minutes</v>
+        <v>21 heures 55 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4375,11 +4423,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>725</v>
+        <v>895</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>1145</v>
+        <v>1315</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5202,100 +5250,178 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="74" t="str">
+      <c r="A39" s="74">
         <f>IF(ISBLANK(B39),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B39))</f>
-        <v/>
-      </c>
-      <c r="B39" s="40"/>
+        <v>51</v>
+      </c>
+      <c r="B39" s="40">
+        <v>46010</v>
+      </c>
       <c r="C39" s="41"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="46"/>
+      <c r="D39" s="42">
+        <v>5</v>
+      </c>
+      <c r="E39" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="G39" s="46" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="73" t="str">
+      <c r="A40" s="73">
         <f>IF(ISBLANK(B40),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B40))</f>
-        <v/>
-      </c>
-      <c r="B40" s="36"/>
+        <v>51</v>
+      </c>
+      <c r="B40" s="36">
+        <v>46010</v>
+      </c>
       <c r="C40" s="37"/>
-      <c r="D40" s="38"/>
+      <c r="D40" s="38">
+        <v>15</v>
+      </c>
       <c r="E40" s="39"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="45"/>
+      <c r="F40" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="G40" s="45" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="74" t="str">
+      <c r="A41" s="74">
         <f>IF(ISBLANK(B41),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B41))</f>
-        <v/>
-      </c>
-      <c r="B41" s="40"/>
+        <v>51</v>
+      </c>
+      <c r="B41" s="40">
+        <v>46010</v>
+      </c>
       <c r="C41" s="41"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="46"/>
+      <c r="D41" s="42">
+        <v>50</v>
+      </c>
+      <c r="E41" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="G41" s="46" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="73" t="str">
+      <c r="A42" s="73">
         <f>IF(ISBLANK(B42),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B42))</f>
-        <v/>
-      </c>
-      <c r="B42" s="36"/>
+        <v>51</v>
+      </c>
+      <c r="B42" s="36">
+        <v>46010</v>
+      </c>
       <c r="C42" s="37"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="45"/>
+      <c r="D42" s="38">
+        <v>20</v>
+      </c>
+      <c r="E42" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="G42" s="45" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="74" t="str">
+      <c r="A43" s="74">
         <f>IF(ISBLANK(B43),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B43))</f>
-        <v/>
-      </c>
-      <c r="B43" s="40"/>
+        <v>51</v>
+      </c>
+      <c r="B43" s="40">
+        <v>46010</v>
+      </c>
       <c r="C43" s="41"/>
-      <c r="D43" s="42"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="46"/>
+      <c r="D43" s="42">
+        <v>35</v>
+      </c>
+      <c r="E43" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="G43" s="46" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="73" t="str">
+      <c r="A44" s="73">
         <f>IF(ISBLANK(B44),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B44))</f>
-        <v/>
-      </c>
-      <c r="B44" s="36"/>
+        <v>51</v>
+      </c>
+      <c r="B44" s="36">
+        <v>46010</v>
+      </c>
       <c r="C44" s="37"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="45"/>
+      <c r="D44" s="38">
+        <v>5</v>
+      </c>
+      <c r="E44" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="G44" s="45" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="74" t="str">
+      <c r="A45" s="74">
         <f>IF(ISBLANK(B45),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B45))</f>
-        <v/>
-      </c>
-      <c r="B45" s="40"/>
+        <v>51</v>
+      </c>
+      <c r="B45" s="40">
+        <v>46010</v>
+      </c>
       <c r="C45" s="41"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="46"/>
+      <c r="D45" s="42">
+        <v>20</v>
+      </c>
+      <c r="E45" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="G45" s="46" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="73" t="str">
+      <c r="A46" s="73">
         <f>IF(ISBLANK(B46),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B46))</f>
-        <v/>
-      </c>
-      <c r="B46" s="36"/>
+        <v>51</v>
+      </c>
+      <c r="B46" s="36">
+        <v>46010</v>
+      </c>
       <c r="C46" s="37"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="45"/>
+      <c r="D46" s="38">
+        <v>20</v>
+      </c>
+      <c r="E46" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="G46" s="45" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="74" t="str">
@@ -11285,7 +11411,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>1.7467248908296942E-2</v>
+        <v>1.5384615384615385E-2</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11306,11 +11432,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>665</v>
+        <v>820</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>1085</v>
+        <v>1240</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11318,11 +11444,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>18 h 05 min</v>
+        <v>20 h 40 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.94759825327510916</v>
+        <v>0.9538461538461539</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11359,7 +11485,7 @@
       </c>
       <c r="G8" s="47">
         <f t="shared" si="2"/>
-        <v>3.4934497816593885E-2</v>
+        <v>3.0769230769230771E-2</v>
       </c>
       <c r="L8" s="65" t="str">
         <f>'Journal de travail'!M10</f>
@@ -11417,22 +11543,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>725</v>
+        <v>880</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>1145</v>
+        <v>1300</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>19 h 05 min</v>
+        <v>21 h 40 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.21685606060606061</v>
+        <v>0.24621212121212122</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
DOC(jdt) jdt du 09.01.2026
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_RubertiGianmarco_Model.xlsx
+++ b/Journal-de-Travail_RubertiGianmarco_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\py13koy\Documents\github\p-bulle-exercices-js-start\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7654E6-27C7-4B8F-8CFD-770214983F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463EDF53-2923-4F37-8920-AE9DADC46864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="114">
   <si>
     <t>Auteur:</t>
   </si>
@@ -359,6 +359,30 @@
   </si>
   <si>
     <t>15h37-15h59</t>
+  </si>
+  <si>
+    <t>train-driver</t>
+  </si>
+  <si>
+    <t>12h38-13h25</t>
+  </si>
+  <si>
+    <t>two-fer</t>
+  </si>
+  <si>
+    <t>13h30-13h36</t>
+  </si>
+  <si>
+    <t>resistor-color</t>
+  </si>
+  <si>
+    <t>14h03-14h09</t>
+  </si>
+  <si>
+    <t>custom-signs</t>
+  </si>
+  <si>
+    <t>14h19-14h39</t>
   </si>
 </sst>
 </file>
@@ -1305,7 +1329,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1240</c:v>
+                  <c:v>1320</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>40</c:v>
@@ -2154,13 +2178,13 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.5384615384615385E-2</c:v>
+                  <c:v>1.4492753623188406E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.9538461538461539</c:v>
+                  <c:v>0.95652173913043481</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0769230769230771E-2</c:v>
+                  <c:v>2.8985507246376812E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -4348,8 +4372,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
+      <pane ySplit="6" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4404,7 +4428,7 @@
       <c r="B3" s="83"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>21 heures 55 minutes</v>
+        <v>23 heures 15 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4423,11 +4447,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>895</v>
+        <v>975</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>1315</v>
+        <v>1395</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -5424,52 +5448,92 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="74" t="str">
+      <c r="A47" s="74">
         <f>IF(ISBLANK(B47),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B47))</f>
-        <v/>
-      </c>
-      <c r="B47" s="40"/>
+        <v>2</v>
+      </c>
+      <c r="B47" s="40">
+        <v>46031</v>
+      </c>
       <c r="C47" s="41"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="46"/>
+      <c r="D47" s="42">
+        <v>50</v>
+      </c>
+      <c r="E47" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="G47" s="46" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="73" t="str">
+      <c r="A48" s="73">
         <f>IF(ISBLANK(B48),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B48))</f>
-        <v/>
-      </c>
-      <c r="B48" s="36"/>
+        <v>2</v>
+      </c>
+      <c r="B48" s="36">
+        <v>46031</v>
+      </c>
       <c r="C48" s="37"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="45"/>
+      <c r="D48" s="38">
+        <v>5</v>
+      </c>
+      <c r="E48" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="G48" s="45" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="74" t="str">
+      <c r="A49" s="74">
         <f>IF(ISBLANK(B49),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B49))</f>
-        <v/>
-      </c>
-      <c r="B49" s="40"/>
+        <v>2</v>
+      </c>
+      <c r="B49" s="40">
+        <v>46031</v>
+      </c>
       <c r="C49" s="41"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="43"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="46"/>
+      <c r="D49" s="42">
+        <v>5</v>
+      </c>
+      <c r="E49" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="G49" s="46" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="73" t="str">
+      <c r="A50" s="73">
         <f>IF(ISBLANK(B50),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B50))</f>
-        <v/>
-      </c>
-      <c r="B50" s="36"/>
+        <v>2</v>
+      </c>
+      <c r="B50" s="36">
+        <v>46031</v>
+      </c>
       <c r="C50" s="37"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="39"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="45"/>
+      <c r="D50" s="38">
+        <v>20</v>
+      </c>
+      <c r="E50" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="G50" s="45" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="74" t="str">
@@ -11411,7 +11475,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>1.5384615384615385E-2</v>
+        <v>1.4492753623188406E-2</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11432,11 +11496,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>820</v>
+        <v>900</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>1240</v>
+        <v>1320</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11444,11 +11508,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>20 h 40 min</v>
+        <v>22 h 00 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.9538461538461539</v>
+        <v>0.95652173913043481</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11485,7 +11549,7 @@
       </c>
       <c r="G8" s="47">
         <f t="shared" si="2"/>
-        <v>3.0769230769230771E-2</v>
+        <v>2.8985507246376812E-2</v>
       </c>
       <c r="L8" s="65" t="str">
         <f>'Journal de travail'!M10</f>
@@ -11543,22 +11607,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>880</v>
+        <v>960</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>1300</v>
+        <v>1380</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>21 h 40 min</v>
+        <v>23 h 00 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.24621212121212122</v>
+        <v>0.26136363636363635</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11602,6 +11666,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="020ab319e6f8d23aec07c29d6516d4ba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e15d3f914bf2a775f9387e5284d9197" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11814,42 +11899,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <img xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6394C10-4386-493D-A99B-15992834CB10}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11868,9 +11921,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6394C10-4386-493D-A99B-15992834CB10}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>